<commit_message>
add ui prototype, update entities
</commit_message>
<xml_diff>
--- a/Entities.xlsx
+++ b/Entities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ErkanMaras.NEBIM\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24AFB48B-E1A3-4B59-910D-26E6774E3F6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A2A944-2F10-499A-B0B7-F3BC68777CC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{586DF947-0067-438E-99FD-7B892C0C1AAC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Guid</t>
   </si>
@@ -100,6 +100,39 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>CustomerId</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Tax</t>
   </si>
 </sst>
 </file>
@@ -461,21 +494,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDFD716-A4CF-4557-B7A6-274DB9F4C7C9}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -491,8 +525,11 @@
       <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -523,8 +560,14 @@
       <c r="N2" t="s">
         <v>0</v>
       </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -532,10 +575,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -544,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
         <v>2</v>
@@ -555,14 +598,26 @@
       <c r="N3" t="s">
         <v>20</v>
       </c>
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
@@ -570,10 +625,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="M4" t="s">
         <v>21</v>
@@ -581,21 +636,79 @@
       <c r="N4" t="s">
         <v>16</v>
       </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
       <c r="G5" t="s">
         <v>15</v>
       </c>
       <c r="H5" t="s">
         <v>16</v>
       </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>